<commit_message>
deleted all IN_DB,WBS test 20180511完了 Signed-off-by: MaHongTao <mht@shequchina.com>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_物件管理_駐車場.xlsx
+++ b/test_物件管理/test_物件管理_駐車場.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\elwj\git\AP\ap2\areaparking-test\test_物件管理\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="13650" tabRatio="850"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="850" firstSheet="7" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="19" r:id="rId1"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="283">
   <si>
     <t>SQL</t>
   </si>
@@ -798,9 +803,6 @@
   </si>
   <si>
     <t>001-001-003</t>
-  </si>
-  <si>
-    <t>IN_DB_003</t>
   </si>
   <si>
     <t>IN_FORM_003</t>
@@ -890,14 +892,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="40">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -909,19 +905,21 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="128"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="DengXian"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -930,12 +928,14 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -964,6 +964,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -983,6 +984,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -990,6 +992,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
@@ -997,6 +1000,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1016,6 +1020,7 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1031,160 +1036,25 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1199,19 +1069,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399945066682943"/>
+        <fgColor theme="7" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399945066682943"/>
+        <fgColor theme="9" tint="0.39991454817346722"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1223,19 +1093,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.4"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.6"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14996795556505"/>
+        <fgColor theme="0" tint="-0.14993743705557422"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1253,7 +1123,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399914548173467"/>
+        <fgColor theme="8" tint="0.39988402966399123"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1263,176 +1133,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1468,254 +1170,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1752,7 +1212,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1785,7 +1245,7 @@
     <xf numFmtId="49" fontId="10" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1814,66 +1274,25 @@
     <xf numFmtId="49" fontId="19" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
+    <cellStyle name="標準 26" xfId="1"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="標準 26" xfId="14"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="15" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="16" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="17" builtinId="11"/>
-    <cellStyle name="标题" xfId="18" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="19" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="20" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="21" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="22" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="23" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="24" builtinId="44"/>
-    <cellStyle name="输出" xfId="25" builtinId="21"/>
-    <cellStyle name="计算" xfId="26" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="27" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="28" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="30" builtinId="24"/>
-    <cellStyle name="汇总" xfId="31" builtinId="25"/>
-    <cellStyle name="好" xfId="32" builtinId="26"/>
-    <cellStyle name="适中" xfId="33" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="34" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="35" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="36" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="37" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="38" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="39" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="40" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="43" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="46" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.249946592608417"/>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1882,6 +1301,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1930,7 +1352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1965,7 +1387,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2168,16 +1590,16 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:BV60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -2189,7 +1611,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="1" ht="14.25" spans="1:8">
+    <row r="3" spans="1:71" customFormat="1" ht="14.25">
       <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
@@ -2203,7 +1625,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" customFormat="1" ht="14.25" spans="1:8">
+    <row r="4" spans="1:71" customFormat="1" ht="14.25">
       <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
@@ -2217,7 +1639,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" customFormat="1" ht="14.25" spans="1:8">
+    <row r="5" spans="1:71" customFormat="1" ht="14.25">
       <c r="A5" s="37" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +1652,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" customFormat="1" ht="14.25" spans="1:8">
+    <row r="6" spans="1:71" customFormat="1" ht="14.25">
       <c r="A6" s="37" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +1666,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" ht="14.25" spans="1:2">
+    <row r="7" spans="1:71" ht="14.25">
       <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
@@ -2252,7 +1674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" ht="14.25" spans="1:7">
+    <row r="8" spans="1:71" ht="14.25">
       <c r="A8" s="32" t="s">
         <v>0</v>
       </c>
@@ -2265,7 +1687,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" ht="14.25" spans="1:7">
+    <row r="9" spans="1:71" ht="14.25">
       <c r="A9" s="32" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +1700,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" ht="14.25" spans="1:7">
+    <row r="10" spans="1:71" ht="14.25">
       <c r="A10" s="32" t="s">
         <v>0</v>
       </c>
@@ -2291,7 +1713,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" ht="14.25" spans="1:7">
+    <row r="11" spans="1:71" ht="14.25">
       <c r="A11" s="32" t="s">
         <v>0</v>
       </c>
@@ -2304,7 +1726,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" ht="14.25" spans="1:7">
+    <row r="12" spans="1:71" ht="14.25">
       <c r="A12" s="32" t="s">
         <v>0</v>
       </c>
@@ -2317,7 +1739,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:71">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -2326,7 +1748,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" customFormat="1" ht="13.5" spans="1:7">
+    <row r="14" spans="1:71" customFormat="1" ht="13.5">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -2335,7 +1757,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="15" spans="1:71" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A15" s="16" t="s">
         <v>11</v>
       </c>
@@ -2343,7 +1765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" s="13" customFormat="1" ht="13.5" spans="2:71">
+    <row r="16" spans="1:71" s="13" customFormat="1" ht="13.5">
       <c r="B16" s="17" t="s">
         <v>13</v>
       </c>
@@ -2417,7 +1839,7 @@
       <c r="BR16" s="18"/>
       <c r="BS16" s="18"/>
     </row>
-    <row r="17" s="13" customFormat="1" ht="13.5" spans="2:74">
+    <row r="17" spans="1:74" s="13" customFormat="1" ht="13.5">
       <c r="B17" s="19" t="s">
         <v>14</v>
       </c>
@@ -2638,7 +2060,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="18" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A18" s="21"/>
       <c r="B18" s="22" t="s">
         <v>87</v>
@@ -2860,7 +2282,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" customFormat="1" ht="13.5" spans="2:74">
+    <row r="19" spans="1:74" customFormat="1" ht="13.5">
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
@@ -2935,7 +2357,7 @@
       <c r="BU19" s="25"/>
       <c r="BV19" s="25"/>
     </row>
-    <row r="20" customFormat="1" ht="13.5" spans="1:7">
+    <row r="20" spans="1:74" customFormat="1" ht="13.5">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -2944,7 +2366,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" customFormat="1" ht="13.5" spans="1:7">
+    <row r="21" spans="1:74" customFormat="1" ht="13.5">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -2953,7 +2375,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" customFormat="1" ht="13.5" spans="1:7">
+    <row r="22" spans="1:74" customFormat="1" ht="13.5">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2962,7 +2384,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" customFormat="1" ht="13.5" spans="1:7">
+    <row r="23" spans="1:74" customFormat="1" ht="13.5">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -2971,7 +2393,7 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="24" spans="1:74" s="14" customFormat="1" ht="14.25">
       <c r="A24" s="32" t="s">
         <v>11</v>
       </c>
@@ -2979,7 +2401,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" s="14" customFormat="1" spans="2:19">
+    <row r="25" spans="1:74" s="14" customFormat="1">
       <c r="B25" s="33" t="s">
         <v>106</v>
       </c>
@@ -3035,7 +2457,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" s="14" customFormat="1" spans="2:19">
+    <row r="26" spans="1:74" s="14" customFormat="1">
       <c r="B26" s="20" t="s">
         <v>108</v>
       </c>
@@ -3091,7 +2513,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" s="14" customFormat="1" spans="2:19">
+    <row r="27" spans="1:74" s="14" customFormat="1">
       <c r="B27" s="23" t="s">
         <v>102</v>
       </c>
@@ -3147,7 +2569,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" s="14" customFormat="1" spans="2:19">
+    <row r="28" spans="1:74" s="14" customFormat="1">
       <c r="B28" s="23" t="s">
         <v>99</v>
       </c>
@@ -3203,7 +2625,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" s="14" customFormat="1" spans="2:19">
+    <row r="29" spans="1:74" s="14" customFormat="1">
       <c r="B29" s="23" t="s">
         <v>126</v>
       </c>
@@ -3259,7 +2681,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" s="14" customFormat="1" spans="2:19">
+    <row r="30" spans="1:74" s="14" customFormat="1">
       <c r="B30" s="23" t="s">
         <v>129</v>
       </c>
@@ -3315,7 +2737,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" s="14" customFormat="1" spans="2:19">
+    <row r="31" spans="1:74" s="14" customFormat="1">
       <c r="B31" s="23" t="s">
         <v>132</v>
       </c>
@@ -3371,7 +2793,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" s="14" customFormat="1" spans="2:19">
+    <row r="32" spans="1:74" s="14" customFormat="1">
       <c r="B32" s="23" t="s">
         <v>104</v>
       </c>
@@ -3427,7 +2849,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" s="14" customFormat="1" spans="2:19">
+    <row r="33" spans="1:19" s="14" customFormat="1">
       <c r="B33" s="23" t="s">
         <v>137</v>
       </c>
@@ -3483,8 +2905,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" s="14" customFormat="1"/>
-    <row r="36" ht="14.25" spans="1:7">
+    <row r="34" spans="1:19" s="14" customFormat="1"/>
+    <row r="36" spans="1:19" ht="14.25">
       <c r="A36" s="32" t="s">
         <v>11</v>
       </c>
@@ -3497,7 +2919,7 @@
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="1:19">
       <c r="B37" s="33" t="s">
         <v>141</v>
       </c>
@@ -3517,7 +2939,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:19">
       <c r="A38" s="14"/>
       <c r="B38" s="20" t="s">
         <v>108</v>
@@ -3538,7 +2960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:19">
       <c r="A39" s="14"/>
       <c r="B39" s="23" t="s">
         <v>102</v>
@@ -3559,7 +2981,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" ht="14.25" spans="1:10">
+    <row r="42" spans="1:19" ht="14.25">
       <c r="A42" s="32" t="s">
         <v>11</v>
       </c>
@@ -3575,7 +2997,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
     </row>
-    <row r="43" spans="2:10">
+    <row r="43" spans="1:19">
       <c r="B43" s="33" t="s">
         <v>144</v>
       </c>
@@ -3604,7 +3026,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:19">
       <c r="A44" s="14"/>
       <c r="B44" s="20" t="s">
         <v>108</v>
@@ -3634,7 +3056,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:19">
       <c r="A45" s="14"/>
       <c r="B45" s="23" t="s">
         <v>102</v>
@@ -3664,7 +3086,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:19">
       <c r="A46" s="14"/>
       <c r="B46" s="23" t="s">
         <v>99</v>
@@ -3694,7 +3116,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:19">
       <c r="A47" s="14"/>
       <c r="B47" s="23" t="s">
         <v>126</v>
@@ -3724,7 +3146,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:19">
       <c r="A48" s="14"/>
       <c r="B48" s="23" t="s">
         <v>129</v>
@@ -3754,7 +3176,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:13">
       <c r="A49" s="14"/>
       <c r="B49" s="23" t="s">
         <v>132</v>
@@ -3784,7 +3206,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:13">
       <c r="A50" s="14"/>
       <c r="B50" s="23" t="s">
         <v>104</v>
@@ -3814,7 +3236,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:13">
       <c r="A51" s="14"/>
       <c r="B51" s="23" t="s">
         <v>137</v>
@@ -3844,7 +3266,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="54" spans="1:13" s="14" customFormat="1" ht="14.25">
       <c r="A54" s="32" t="s">
         <v>11</v>
       </c>
@@ -3852,7 +3274,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" s="14" customFormat="1" spans="2:13">
+    <row r="55" spans="1:13" s="14" customFormat="1">
       <c r="B55" s="33" t="s">
         <v>150</v>
       </c>
@@ -3890,7 +3312,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" s="14" customFormat="1" spans="2:13">
+    <row r="56" spans="1:13" s="14" customFormat="1">
       <c r="B56" s="20" t="s">
         <v>108</v>
       </c>
@@ -3928,7 +3350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" s="14" customFormat="1" spans="2:13">
+    <row r="57" spans="1:13" s="14" customFormat="1">
       <c r="B57" s="23" t="s">
         <v>102</v>
       </c>
@@ -3966,7 +3388,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" s="14" customFormat="1" spans="2:13">
+    <row r="58" spans="1:13" s="14" customFormat="1">
       <c r="B58" s="23" t="s">
         <v>99</v>
       </c>
@@ -4004,7 +3426,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" s="14" customFormat="1" spans="2:13">
+    <row r="59" spans="1:13" s="14" customFormat="1">
       <c r="B59" s="23" t="s">
         <v>126</v>
       </c>
@@ -4042,29 +3464,28 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" s="14" customFormat="1"/>
+    <row r="60" spans="1:13" s="14" customFormat="1"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -4072,7 +3493,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -4146,7 +3567,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -4367,7 +3788,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -4589,7 +4010,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -4664,17 +4085,16 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" s="14" customFormat="1" ht="12"/>
-    <row r="8" s="15" customFormat="1" ht="12"/>
+    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
+    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S44"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4690,7 +4110,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="2" ht="14.25" spans="1:7">
+    <row r="2" spans="1:19" ht="14.25">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -4703,7 +4123,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" ht="14.25" spans="1:7">
+    <row r="3" spans="1:19" ht="14.25">
       <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
@@ -4716,7 +4136,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" ht="14.25" spans="1:7">
+    <row r="4" spans="1:19" ht="14.25">
       <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
@@ -4729,7 +4149,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" ht="14.25" spans="1:7">
+    <row r="5" spans="1:19" ht="14.25">
       <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
@@ -4742,7 +4162,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" ht="14.25" spans="1:7">
+    <row r="6" spans="1:19" ht="14.25">
       <c r="A6" s="32" t="s">
         <v>0</v>
       </c>
@@ -4755,7 +4175,7 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:19">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -4764,7 +4184,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="8" spans="1:19" s="14" customFormat="1" ht="14.25">
       <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
@@ -4772,7 +4192,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" s="14" customFormat="1" spans="2:19">
+    <row r="9" spans="1:19" s="14" customFormat="1">
       <c r="B9" s="33" t="s">
         <v>106</v>
       </c>
@@ -4828,7 +4248,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" s="14" customFormat="1" spans="2:19">
+    <row r="10" spans="1:19" s="14" customFormat="1">
       <c r="B10" s="20" t="s">
         <v>108</v>
       </c>
@@ -4884,7 +4304,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" s="14" customFormat="1" spans="2:19">
+    <row r="11" spans="1:19" s="14" customFormat="1">
       <c r="B11" s="23" t="s">
         <v>102</v>
       </c>
@@ -4940,7 +4360,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" s="14" customFormat="1" spans="2:19">
+    <row r="12" spans="1:19" s="14" customFormat="1">
       <c r="B12" s="23" t="s">
         <v>99</v>
       </c>
@@ -4996,7 +4416,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" s="14" customFormat="1" spans="2:19">
+    <row r="13" spans="1:19" s="14" customFormat="1">
       <c r="B13" s="23" t="s">
         <v>126</v>
       </c>
@@ -5052,7 +4472,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" s="14" customFormat="1" spans="2:19">
+    <row r="14" spans="1:19" s="14" customFormat="1">
       <c r="B14" s="23" t="s">
         <v>129</v>
       </c>
@@ -5108,7 +4528,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" s="14" customFormat="1" spans="2:19">
+    <row r="15" spans="1:19" s="14" customFormat="1">
       <c r="B15" s="23" t="s">
         <v>132</v>
       </c>
@@ -5164,7 +4584,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" s="14" customFormat="1" spans="2:19">
+    <row r="16" spans="1:19" s="14" customFormat="1">
       <c r="B16" s="23" t="s">
         <v>104</v>
       </c>
@@ -5220,7 +4640,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" s="14" customFormat="1" spans="2:19">
+    <row r="17" spans="1:19" s="14" customFormat="1">
       <c r="B17" s="23" t="s">
         <v>137</v>
       </c>
@@ -5276,8 +4696,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="1"/>
-    <row r="20" ht="14.25" spans="1:7">
+    <row r="18" spans="1:19" s="14" customFormat="1"/>
+    <row r="20" spans="1:19" ht="14.25">
       <c r="A20" s="32" t="s">
         <v>11</v>
       </c>
@@ -5290,7 +4710,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="1:19">
       <c r="B21" s="33" t="s">
         <v>141</v>
       </c>
@@ -5310,7 +4730,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:19">
       <c r="A22" s="14"/>
       <c r="B22" s="20" t="s">
         <v>108</v>
@@ -5331,7 +4751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:19">
       <c r="A23" s="14"/>
       <c r="B23" s="23" t="s">
         <v>102</v>
@@ -5352,7 +4772,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" ht="14.25" spans="1:10">
+    <row r="26" spans="1:19" ht="14.25">
       <c r="A26" s="32" t="s">
         <v>11</v>
       </c>
@@ -5368,7 +4788,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="1:19">
       <c r="B27" s="33" t="s">
         <v>144</v>
       </c>
@@ -5397,7 +4817,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:19">
       <c r="A28" s="14"/>
       <c r="B28" s="20" t="s">
         <v>108</v>
@@ -5427,7 +4847,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:19">
       <c r="A29" s="14"/>
       <c r="B29" s="23" t="s">
         <v>102</v>
@@ -5457,7 +4877,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:19">
       <c r="A30" s="14"/>
       <c r="B30" s="23" t="s">
         <v>99</v>
@@ -5487,7 +4907,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:19">
       <c r="A31" s="14"/>
       <c r="B31" s="23" t="s">
         <v>126</v>
@@ -5517,7 +4937,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:19">
       <c r="A32" s="14"/>
       <c r="B32" s="23" t="s">
         <v>129</v>
@@ -5547,7 +4967,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:13">
       <c r="A33" s="14"/>
       <c r="B33" s="23" t="s">
         <v>132</v>
@@ -5577,7 +4997,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:13">
       <c r="A34" s="14"/>
       <c r="B34" s="23" t="s">
         <v>104</v>
@@ -5607,7 +5027,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:13">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
         <v>137</v>
@@ -5637,7 +5057,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="38" spans="1:13" s="14" customFormat="1" ht="14.25">
       <c r="A38" s="32" t="s">
         <v>11</v>
       </c>
@@ -5645,7 +5065,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" s="14" customFormat="1" spans="2:13">
+    <row r="39" spans="1:13" s="14" customFormat="1">
       <c r="B39" s="33" t="s">
         <v>150</v>
       </c>
@@ -5683,7 +5103,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" s="14" customFormat="1" spans="2:13">
+    <row r="40" spans="1:13" s="14" customFormat="1">
       <c r="B40" s="20" t="s">
         <v>108</v>
       </c>
@@ -5721,7 +5141,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" s="14" customFormat="1" spans="2:13">
+    <row r="41" spans="1:13" s="14" customFormat="1">
       <c r="B41" s="23" t="s">
         <v>102</v>
       </c>
@@ -5759,7 +5179,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" s="14" customFormat="1" spans="2:13">
+    <row r="42" spans="1:13" s="14" customFormat="1">
       <c r="B42" s="23" t="s">
         <v>99</v>
       </c>
@@ -5797,7 +5217,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" s="14" customFormat="1" spans="2:13">
+    <row r="43" spans="1:13" s="14" customFormat="1">
       <c r="B43" s="23" t="s">
         <v>126</v>
       </c>
@@ -5835,24 +5255,23 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" s="14" customFormat="1"/>
+    <row r="44" spans="1:13" s="14" customFormat="1"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -5862,7 +5281,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:5" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -5870,7 +5289,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:5" ht="12" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -5878,7 +5297,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:2">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -5886,14 +5305,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="13.5" spans="1:5">
+    <row r="7" spans="1:5" customFormat="1" ht="13.5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" ht="14.25" spans="1:2">
+    <row r="9" spans="1:5" ht="14.25">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -5901,7 +5320,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" s="15" customFormat="1" customHeight="1" spans="1:2">
+    <row r="12" spans="1:5" ht="12" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>166</v>
       </c>
@@ -5910,27 +5329,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -5938,7 +5356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -6012,7 +5430,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -6233,7 +5651,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -6455,7 +5873,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -6530,24 +5948,23 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" s="14" customFormat="1" ht="12"/>
-    <row r="8" s="15" customFormat="1" ht="12"/>
+    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
+    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="$A13:$XFD13"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -6557,7 +5974,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:5" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -6565,7 +5982,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:5" ht="12" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -6573,7 +5990,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:2">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -6581,14 +5998,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="13.5" spans="1:5">
+    <row r="7" spans="1:5" customFormat="1" ht="13.5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" ht="14.25" spans="1:2">
+    <row r="9" spans="1:5" ht="14.25">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -6596,7 +6013,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" s="15" customFormat="1" customHeight="1" spans="1:2">
+    <row r="12" spans="1:5" ht="12" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>166</v>
       </c>
@@ -6604,10 +6021,10 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" ht="14.25" spans="1:1">
+    <row r="13" spans="1:5" ht="14.25">
       <c r="A13" s="27"/>
     </row>
-    <row r="16" ht="14.25" spans="1:2">
+    <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="27" t="s">
         <v>186</v>
       </c>
@@ -6615,7 +6032,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" ht="14.25" spans="1:4">
+    <row r="17" spans="1:4" ht="14.25">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
         <v>178</v>
@@ -6627,7 +6044,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" ht="14.25" spans="1:4">
+    <row r="18" spans="1:4" ht="14.25">
       <c r="A18" s="27" t="s">
         <v>188</v>
       </c>
@@ -6641,7 +6058,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" ht="14.25" spans="1:2">
+    <row r="22" spans="1:4" ht="14.25">
       <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
@@ -6650,27 +6067,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -6678,7 +6094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -6752,7 +6168,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -6973,7 +6389,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -7195,7 +6611,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -7270,24 +6686,23 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" s="14" customFormat="1" ht="12"/>
-    <row r="8" s="15" customFormat="1" ht="12"/>
+    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
+    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="$A13:$XFD13"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -7297,7 +6712,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:5" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -7305,7 +6720,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:5" ht="12" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -7313,7 +6728,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:2">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -7321,14 +6736,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="13.5" spans="1:5">
+    <row r="7" spans="1:5" customFormat="1" ht="13.5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" ht="14.25" spans="1:2">
+    <row r="9" spans="1:5" ht="14.25">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -7336,7 +6751,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" s="15" customFormat="1" customHeight="1" spans="1:2">
+    <row r="12" spans="1:5" ht="12" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>166</v>
       </c>
@@ -7344,10 +6759,10 @@
         <v>231</v>
       </c>
     </row>
-    <row r="13" s="15" customFormat="1" ht="14.25" spans="1:1">
+    <row r="13" spans="1:5" ht="14.25">
       <c r="A13" s="27"/>
     </row>
-    <row r="16" s="15" customFormat="1" ht="14.25" spans="1:2">
+    <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="27" t="s">
         <v>186</v>
       </c>
@@ -7355,7 +6770,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" s="15" customFormat="1" ht="14.25" spans="1:4">
+    <row r="17" spans="1:4" ht="14.25">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
         <v>178</v>
@@ -7367,7 +6782,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" s="15" customFormat="1" ht="14.25" spans="1:4">
+    <row r="18" spans="1:4" ht="14.25">
       <c r="A18" s="27" t="s">
         <v>188</v>
       </c>
@@ -7381,7 +6796,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" s="15" customFormat="1" ht="14.25" spans="1:2">
+    <row r="22" spans="1:4" ht="14.25">
       <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
@@ -7390,27 +6805,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U52" sqref="U52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -7418,7 +6832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -7492,7 +6906,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -7713,7 +7127,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -7935,7 +7349,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -8010,24 +7424,23 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" s="14" customFormat="1" ht="12"/>
-    <row r="8" s="15" customFormat="1" ht="12"/>
+    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
+    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -8037,7 +7450,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:5" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -8045,7 +7458,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:5" ht="12" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -8053,7 +7466,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:2">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -8061,7 +7474,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="13.5" spans="1:5">
+    <row r="7" spans="1:5" customFormat="1" ht="13.5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -8069,27 +7482,26 @@
       <c r="E7" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -8097,7 +7509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -8171,7 +7583,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -8392,7 +7804,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -8614,7 +8026,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -8689,24 +8101,23 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" s="14" customFormat="1" ht="12"/>
-    <row r="8" s="15" customFormat="1" ht="12"/>
+    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
+    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -8716,7 +8127,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:5" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -8724,7 +8135,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:5" ht="12" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -8732,7 +8143,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:2">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -8740,7 +8151,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="13.5" spans="1:5">
+    <row r="7" spans="1:5" customFormat="1" ht="13.5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -8748,19 +8159,18 @@
       <c r="E7" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -8847,71 +8257,68 @@
       <c r="B7" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="12" t="s">
@@ -8920,45 +8327,46 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="I12" s="10" t="s">
         <v>282</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>283</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>248</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="I5:J5">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$M5="完了"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8967,27 +8375,25 @@
       <formula>$M12="完了"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -8995,7 +8401,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -9069,7 +8475,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -9290,7 +8696,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -9512,7 +8918,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -9587,24 +8993,23 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" s="14" customFormat="1" ht="12"/>
-    <row r="8" s="15" customFormat="1" ht="12"/>
+    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
+    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -9614,7 +9019,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:5" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -9622,7 +9027,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:5" ht="12" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -9630,7 +9035,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:2">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -9638,14 +9043,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="13.5" spans="1:5">
+    <row r="7" spans="1:5" customFormat="1" ht="13.5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" ht="14.25" spans="1:2">
+    <row r="9" spans="1:5" ht="14.25">
       <c r="A9" s="27" t="s">
         <v>176</v>
       </c>
@@ -9653,7 +9058,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="10" spans="1:5" ht="12" customHeight="1">
       <c r="A10" s="27"/>
       <c r="B10" s="28" t="s">
         <v>178</v>
@@ -9665,7 +9070,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="11" spans="1:5" ht="12" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>181</v>
       </c>
@@ -9679,7 +9084,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" s="15" customFormat="1" customHeight="1" spans="1:2">
+    <row r="14" spans="1:5" ht="12" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>166</v>
       </c>
@@ -9688,27 +9093,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -9716,7 +9120,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -9790,7 +9194,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -10011,7 +9415,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -10233,7 +9637,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -10308,21 +9712,20 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" s="14" customFormat="1" ht="12"/>
-    <row r="8" s="15" customFormat="1" ht="12"/>
+    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
+    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="$A1:$XFD3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -10334,7 +9737,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="1" ht="14.25" spans="1:8">
+    <row r="3" spans="1:19" customFormat="1" ht="14.25">
       <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
@@ -10348,7 +9751,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" customFormat="1" ht="14.25" spans="1:8">
+    <row r="4" spans="1:19" customFormat="1" ht="14.25">
       <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
@@ -10362,7 +9765,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" customFormat="1" ht="14.25" spans="1:8">
+    <row r="5" spans="1:19" customFormat="1" ht="14.25">
       <c r="A5" s="37" t="s">
         <v>0</v>
       </c>
@@ -10375,7 +9778,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" customFormat="1" ht="14.25" spans="1:8">
+    <row r="6" spans="1:19" customFormat="1" ht="14.25">
       <c r="A6" s="37" t="s">
         <v>0</v>
       </c>
@@ -10389,7 +9792,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" ht="14.25" spans="1:2">
+    <row r="7" spans="1:19" ht="14.25">
       <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
@@ -10397,10 +9800,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" ht="14.25" spans="1:7">
-      <c r="A8" s="32" t="s">
-        <v>0</v>
-      </c>
+    <row r="8" spans="1:19" ht="14.25">
+      <c r="A8" s="32"/>
       <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
@@ -10410,7 +9811,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" ht="14.25" spans="1:7">
+    <row r="9" spans="1:19" ht="14.25">
       <c r="A9" s="32" t="s">
         <v>0</v>
       </c>
@@ -10423,7 +9824,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" ht="14.25" spans="1:7">
+    <row r="10" spans="1:19" ht="14.25">
       <c r="A10" s="32" t="s">
         <v>0</v>
       </c>
@@ -10436,7 +9837,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" ht="14.25" spans="1:7">
+    <row r="11" spans="1:19" ht="14.25">
       <c r="A11" s="32" t="s">
         <v>0</v>
       </c>
@@ -10449,7 +9850,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" ht="14.25" spans="1:7">
+    <row r="12" spans="1:19" ht="14.25">
       <c r="A12" s="32" t="s">
         <v>0</v>
       </c>
@@ -10462,7 +9863,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:19">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -10471,7 +9872,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="14" spans="1:19" s="14" customFormat="1" ht="14.25">
       <c r="A14" s="32" t="s">
         <v>11</v>
       </c>
@@ -10479,7 +9880,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" s="14" customFormat="1" spans="2:19">
+    <row r="15" spans="1:19" s="14" customFormat="1">
       <c r="B15" s="33" t="s">
         <v>106</v>
       </c>
@@ -10535,7 +9936,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" s="14" customFormat="1" spans="2:19">
+    <row r="16" spans="1:19" s="14" customFormat="1">
       <c r="B16" s="20" t="s">
         <v>108</v>
       </c>
@@ -10591,7 +9992,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" s="14" customFormat="1" spans="2:19">
+    <row r="17" spans="1:19" s="14" customFormat="1">
       <c r="B17" s="23" t="s">
         <v>102</v>
       </c>
@@ -10647,7 +10048,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="1" spans="2:19">
+    <row r="18" spans="1:19" s="14" customFormat="1">
       <c r="B18" s="23" t="s">
         <v>99</v>
       </c>
@@ -10703,7 +10104,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" s="14" customFormat="1" spans="2:19">
+    <row r="19" spans="1:19" s="14" customFormat="1">
       <c r="B19" s="23" t="s">
         <v>126</v>
       </c>
@@ -10759,7 +10160,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" s="14" customFormat="1" spans="2:19">
+    <row r="20" spans="1:19" s="14" customFormat="1">
       <c r="B20" s="23" t="s">
         <v>129</v>
       </c>
@@ -10815,7 +10216,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" s="14" customFormat="1" spans="2:19">
+    <row r="21" spans="1:19" s="14" customFormat="1">
       <c r="B21" s="23" t="s">
         <v>132</v>
       </c>
@@ -10871,7 +10272,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" s="14" customFormat="1" spans="2:19">
+    <row r="22" spans="1:19" s="14" customFormat="1">
       <c r="B22" s="23" t="s">
         <v>104</v>
       </c>
@@ -10927,7 +10328,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" s="14" customFormat="1" spans="2:19">
+    <row r="23" spans="1:19" s="14" customFormat="1">
       <c r="B23" s="23" t="s">
         <v>137</v>
       </c>
@@ -10983,8 +10384,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" s="14" customFormat="1"/>
-    <row r="26" ht="14.25" spans="1:7">
+    <row r="24" spans="1:19" s="14" customFormat="1"/>
+    <row r="26" spans="1:19" ht="14.25">
       <c r="A26" s="32" t="s">
         <v>11</v>
       </c>
@@ -10997,7 +10398,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="1:19">
       <c r="B27" s="33" t="s">
         <v>141</v>
       </c>
@@ -11017,7 +10418,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:19">
       <c r="A28" s="14"/>
       <c r="B28" s="20" t="s">
         <v>108</v>
@@ -11038,7 +10439,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:19">
       <c r="A29" s="14"/>
       <c r="B29" s="23" t="s">
         <v>102</v>
@@ -11059,7 +10460,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" ht="14.25" spans="1:10">
+    <row r="32" spans="1:19" ht="14.25">
       <c r="A32" s="32" t="s">
         <v>11</v>
       </c>
@@ -11075,7 +10476,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" spans="1:13">
       <c r="B33" s="33" t="s">
         <v>144</v>
       </c>
@@ -11104,7 +10505,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:13">
       <c r="A34" s="14"/>
       <c r="B34" s="20" t="s">
         <v>108</v>
@@ -11134,7 +10535,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:13">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
         <v>102</v>
@@ -11164,7 +10565,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:13">
       <c r="A36" s="14"/>
       <c r="B36" s="23" t="s">
         <v>99</v>
@@ -11194,7 +10595,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:13">
       <c r="A37" s="14"/>
       <c r="B37" s="23" t="s">
         <v>126</v>
@@ -11224,7 +10625,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:13">
       <c r="A38" s="14"/>
       <c r="B38" s="23" t="s">
         <v>129</v>
@@ -11254,7 +10655,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:13">
       <c r="A39" s="14"/>
       <c r="B39" s="23" t="s">
         <v>132</v>
@@ -11284,7 +10685,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:13">
       <c r="A40" s="14"/>
       <c r="B40" s="23" t="s">
         <v>104</v>
@@ -11314,7 +10715,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:13">
       <c r="A41" s="14"/>
       <c r="B41" s="23" t="s">
         <v>137</v>
@@ -11344,7 +10745,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="44" spans="1:13" s="14" customFormat="1" ht="14.25">
       <c r="A44" s="32" t="s">
         <v>11</v>
       </c>
@@ -11352,7 +10753,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" s="14" customFormat="1" spans="2:13">
+    <row r="45" spans="1:13" s="14" customFormat="1">
       <c r="B45" s="33" t="s">
         <v>150</v>
       </c>
@@ -11390,7 +10791,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" s="14" customFormat="1" spans="2:13">
+    <row r="46" spans="1:13" s="14" customFormat="1">
       <c r="B46" s="20" t="s">
         <v>108</v>
       </c>
@@ -11428,7 +10829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" s="14" customFormat="1" spans="2:13">
+    <row r="47" spans="1:13" s="14" customFormat="1">
       <c r="B47" s="23" t="s">
         <v>102</v>
       </c>
@@ -11466,7 +10867,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" s="14" customFormat="1" spans="2:13">
+    <row r="48" spans="1:13" s="14" customFormat="1">
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
@@ -11504,7 +10905,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" s="14" customFormat="1" spans="2:13">
+    <row r="49" spans="2:13" s="14" customFormat="1">
       <c r="B49" s="23" t="s">
         <v>126</v>
       </c>
@@ -11542,24 +10943,23 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" s="14" customFormat="1"/>
+    <row r="50" spans="2:13" s="14" customFormat="1"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="A34 C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -11569,7 +10969,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:4" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -11577,7 +10977,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" customHeight="1" spans="1:2">
+    <row r="3" spans="1:4" ht="12" customHeight="1">
       <c r="A3" s="27" t="s">
         <v>186</v>
       </c>
@@ -11585,7 +10985,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:4">
+    <row r="4" spans="1:4" ht="12" customHeight="1">
       <c r="A4" s="27"/>
       <c r="B4" s="28" t="s">
         <v>178</v>
@@ -11597,7 +10997,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:4">
+    <row r="5" spans="1:4" ht="12" customHeight="1">
       <c r="A5" s="27" t="s">
         <v>188</v>
       </c>
@@ -11611,7 +11011,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" customHeight="1" spans="1:4">
+    <row r="6" spans="1:4" ht="12" customHeight="1">
       <c r="A6" s="27" t="s">
         <v>188</v>
       </c>
@@ -11625,7 +11025,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="7" customHeight="1" spans="1:4">
+    <row r="7" spans="1:4" ht="12" customHeight="1">
       <c r="A7" s="27" t="s">
         <v>188</v>
       </c>
@@ -11637,7 +11037,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="8" customHeight="1" spans="1:4">
+    <row r="8" spans="1:4" ht="12" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>188</v>
       </c>
@@ -11651,7 +11051,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" customHeight="1" spans="1:4">
+    <row r="9" spans="1:4" ht="12" customHeight="1">
       <c r="A9" s="27" t="s">
         <v>188</v>
       </c>
@@ -11665,7 +11065,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" customHeight="1" spans="1:4">
+    <row r="10" spans="1:4" ht="12" customHeight="1">
       <c r="A10" s="27" t="s">
         <v>188</v>
       </c>
@@ -11679,7 +11079,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" customHeight="1" spans="1:4">
+    <row r="11" spans="1:4" ht="12" customHeight="1">
       <c r="A11" s="27" t="s">
         <v>188</v>
       </c>
@@ -11693,7 +11093,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" customHeight="1" spans="1:4">
+    <row r="12" spans="1:4" ht="12" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>188</v>
       </c>
@@ -11707,7 +11107,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" customHeight="1" spans="1:4">
+    <row r="13" spans="1:4" ht="12" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>188</v>
       </c>
@@ -11721,7 +11121,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" customHeight="1" spans="1:4">
+    <row r="14" spans="1:4" ht="12" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>188</v>
       </c>
@@ -11735,7 +11135,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" customHeight="1" spans="1:4">
+    <row r="15" spans="1:4" ht="12" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>188</v>
       </c>
@@ -11749,7 +11149,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" customHeight="1" spans="1:4">
+    <row r="16" spans="1:4" ht="12" customHeight="1">
       <c r="A16" s="27" t="s">
         <v>188</v>
       </c>
@@ -11763,7 +11163,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" customHeight="1" spans="1:3">
+    <row r="17" spans="1:3" ht="12" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>188</v>
       </c>
@@ -11774,7 +11174,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" customHeight="1" spans="1:2">
+    <row r="22" spans="1:3" ht="12" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
@@ -11783,19 +11183,18 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BV45"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD6"/>
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -11803,7 +11202,7 @@
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
+    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -11811,7 +11210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" s="13" customFormat="1" spans="2:71">
+    <row r="3" spans="1:74" s="13" customFormat="1">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -11885,7 +11284,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" s="13" customFormat="1" spans="2:74">
+    <row r="4" spans="1:74" s="13" customFormat="1">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -12106,7 +11505,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
+    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>87</v>
@@ -12328,7 +11727,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:74">
+    <row r="6" spans="1:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -12403,7 +11802,7 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="8" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="8" spans="1:74" s="14" customFormat="1" ht="14.25">
       <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
@@ -12411,7 +11810,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="9" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B9" s="33" t="s">
         <v>204</v>
       </c>
@@ -12467,7 +11866,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="10" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B10" s="20" t="s">
         <v>108</v>
       </c>
@@ -12523,7 +11922,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="11" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B11" s="23" t="s">
         <v>102</v>
       </c>
@@ -12579,7 +11978,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="12" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B12" s="23" t="s">
         <v>99</v>
       </c>
@@ -12635,7 +12034,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="13" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B13" s="23" t="s">
         <v>126</v>
       </c>
@@ -12691,7 +12090,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="14" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B14" s="23" t="s">
         <v>129</v>
       </c>
@@ -12747,7 +12146,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="15" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B15" s="23" t="s">
         <v>132</v>
       </c>
@@ -12803,7 +12202,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="16" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B16" s="23" t="s">
         <v>104</v>
       </c>
@@ -12859,7 +12258,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" s="14" customFormat="1" ht="12" spans="2:19">
+    <row r="17" spans="1:19" s="14" customFormat="1" ht="12">
       <c r="B17" s="23" t="s">
         <v>137</v>
       </c>
@@ -12915,9 +12314,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="1" ht="12"/>
-    <row r="19" s="15" customFormat="1" ht="12"/>
-    <row r="20" s="15" customFormat="1" ht="14.25" spans="1:7">
+    <row r="18" spans="1:19" s="14" customFormat="1" ht="12"/>
+    <row r="19" spans="1:19" s="15" customFormat="1" ht="12"/>
+    <row r="20" spans="1:19" s="15" customFormat="1" ht="14.25">
       <c r="A20" s="32" t="s">
         <v>11</v>
       </c>
@@ -12930,7 +12329,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" s="15" customFormat="1" ht="12" spans="2:7">
+    <row r="21" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="B21" s="33" t="s">
         <v>207</v>
       </c>
@@ -12950,7 +12349,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" s="15" customFormat="1" ht="12" spans="1:7">
+    <row r="22" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="A22" s="14"/>
       <c r="B22" s="20" t="s">
         <v>108</v>
@@ -12971,7 +12370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" s="15" customFormat="1" ht="12" spans="1:7">
+    <row r="23" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="A23" s="14"/>
       <c r="B23" s="23" t="s">
         <v>102</v>
@@ -12992,9 +12391,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" s="15" customFormat="1" ht="12"/>
-    <row r="25" s="15" customFormat="1" ht="12"/>
-    <row r="26" s="15" customFormat="1" ht="14.25" spans="1:10">
+    <row r="24" spans="1:19" s="15" customFormat="1" ht="12"/>
+    <row r="25" spans="1:19" s="15" customFormat="1" ht="12"/>
+    <row r="26" spans="1:19" s="15" customFormat="1" ht="14.25">
       <c r="A26" s="32" t="s">
         <v>11</v>
       </c>
@@ -13010,7 +12409,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" s="15" customFormat="1" ht="12" spans="2:10">
+    <row r="27" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="B27" s="33" t="s">
         <v>208</v>
       </c>
@@ -13039,7 +12438,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="28" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="A28" s="14"/>
       <c r="B28" s="20" t="s">
         <v>108</v>
@@ -13069,7 +12468,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="29" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="A29" s="14"/>
       <c r="B29" s="23" t="s">
         <v>102</v>
@@ -13099,7 +12498,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="30" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="A30" s="14"/>
       <c r="B30" s="23" t="s">
         <v>99</v>
@@ -13129,7 +12528,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="31" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="A31" s="14"/>
       <c r="B31" s="23" t="s">
         <v>126</v>
@@ -13159,7 +12558,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="32" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="A32" s="14"/>
       <c r="B32" s="23" t="s">
         <v>129</v>
@@ -13189,7 +12588,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="33" spans="1:13" s="15" customFormat="1" ht="12">
       <c r="A33" s="14"/>
       <c r="B33" s="23" t="s">
         <v>132</v>
@@ -13219,7 +12618,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="34" spans="1:13" s="15" customFormat="1" ht="12">
       <c r="A34" s="14"/>
       <c r="B34" s="23" t="s">
         <v>104</v>
@@ -13249,7 +12648,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" s="15" customFormat="1" ht="12" spans="1:10">
+    <row r="35" spans="1:13" s="15" customFormat="1" ht="12">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
         <v>137</v>
@@ -13279,9 +12678,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" s="15" customFormat="1" ht="12"/>
-    <row r="37" s="15" customFormat="1" ht="12"/>
-    <row r="38" s="14" customFormat="1" ht="14.25" spans="1:2">
+    <row r="36" spans="1:13" s="15" customFormat="1" ht="12"/>
+    <row r="37" spans="1:13" s="15" customFormat="1" ht="12"/>
+    <row r="38" spans="1:13" s="14" customFormat="1" ht="14.25">
       <c r="A38" s="32" t="s">
         <v>11</v>
       </c>
@@ -13289,7 +12688,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" s="14" customFormat="1" ht="12" spans="2:13">
+    <row r="39" spans="1:13" s="14" customFormat="1" ht="12">
       <c r="B39" s="33" t="s">
         <v>210</v>
       </c>
@@ -13327,7 +12726,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" s="14" customFormat="1" ht="12" spans="2:13">
+    <row r="40" spans="1:13" s="14" customFormat="1" ht="12">
       <c r="B40" s="20" t="s">
         <v>108</v>
       </c>
@@ -13365,7 +12764,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" s="14" customFormat="1" ht="12" spans="2:13">
+    <row r="41" spans="1:13" s="14" customFormat="1" ht="12">
       <c r="B41" s="23" t="s">
         <v>102</v>
       </c>
@@ -13403,7 +12802,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" s="14" customFormat="1" ht="12" spans="2:13">
+    <row r="42" spans="1:13" s="14" customFormat="1" ht="12">
       <c r="B42" s="23" t="s">
         <v>99</v>
       </c>
@@ -13441,7 +12840,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" s="14" customFormat="1" ht="12" spans="2:13">
+    <row r="43" spans="1:13" s="14" customFormat="1" ht="12">
       <c r="B43" s="23" t="s">
         <v>126</v>
       </c>
@@ -13479,24 +12878,23 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" s="14" customFormat="1" ht="12"/>
-    <row r="45" s="15" customFormat="1" ht="12"/>
+    <row r="44" spans="1:13" s="14" customFormat="1" ht="12"/>
+    <row r="45" spans="1:13" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -13506,7 +12904,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" spans="1:5" ht="12" customHeight="1">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
@@ -13514,7 +12912,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:2">
+    <row r="4" spans="1:5" ht="12" customHeight="1">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -13522,7 +12920,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:2">
+    <row r="5" spans="1:5" ht="14.25">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -13530,14 +12928,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" customFormat="1" ht="13.5" spans="1:5">
+    <row r="7" spans="1:5" customFormat="1" ht="13.5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" ht="14.25" spans="1:2">
+    <row r="9" spans="1:5" ht="14.25">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -13545,7 +12943,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" s="15" customFormat="1" customHeight="1" spans="1:2">
+    <row r="12" spans="1:5" ht="12" customHeight="1">
       <c r="A12" s="27" t="s">
         <v>186</v>
       </c>
@@ -13553,7 +12951,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="13" spans="1:5" ht="12" customHeight="1">
       <c r="A13" s="27"/>
       <c r="B13" s="28" t="s">
         <v>178</v>
@@ -13565,7 +12963,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="14" spans="1:5" ht="12" customHeight="1">
       <c r="A14" s="27" t="s">
         <v>188</v>
       </c>
@@ -13579,7 +12977,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="15" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="15" spans="1:5" ht="12" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>188</v>
       </c>
@@ -13593,7 +12991,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="16" spans="1:5" ht="12" customHeight="1">
       <c r="A16" s="27" t="s">
         <v>188</v>
       </c>
@@ -13605,7 +13003,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="17" spans="1:4" ht="12" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>188</v>
       </c>
@@ -13619,7 +13017,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="18" spans="1:4" ht="12" customHeight="1">
       <c r="A18" s="27" t="s">
         <v>188</v>
       </c>
@@ -13633,7 +13031,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="19" spans="1:4" ht="12" customHeight="1">
       <c r="A19" s="27" t="s">
         <v>188</v>
       </c>
@@ -13647,7 +13045,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="20" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="20" spans="1:4" ht="12" customHeight="1">
       <c r="A20" s="27" t="s">
         <v>188</v>
       </c>
@@ -13661,7 +13059,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="21" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="21" spans="1:4" ht="12" customHeight="1">
       <c r="A21" s="27" t="s">
         <v>188</v>
       </c>
@@ -13675,7 +13073,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="22" spans="1:4" ht="12" customHeight="1">
       <c r="A22" s="27" t="s">
         <v>188</v>
       </c>
@@ -13689,7 +13087,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="23" spans="1:4" ht="12" customHeight="1">
       <c r="A23" s="27" t="s">
         <v>188</v>
       </c>
@@ -13703,7 +13101,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="24" spans="1:4" ht="12" customHeight="1">
       <c r="A24" s="27" t="s">
         <v>188</v>
       </c>
@@ -13717,7 +13115,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" s="15" customFormat="1" customHeight="1" spans="1:4">
+    <row r="25" spans="1:4" ht="12" customHeight="1">
       <c r="A25" s="27" t="s">
         <v>188</v>
       </c>
@@ -13731,7 +13129,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" s="15" customFormat="1" customHeight="1" spans="1:3">
+    <row r="26" spans="1:4" ht="12" customHeight="1">
       <c r="A26" s="27" t="s">
         <v>188</v>
       </c>
@@ -13742,7 +13140,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="30" s="15" customFormat="1" customHeight="1" spans="1:2">
+    <row r="30" spans="1:4" ht="12" customHeight="1">
       <c r="A30" s="27" t="s">
         <v>166</v>
       </c>
@@ -13750,7 +13148,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" s="15" customFormat="1" ht="14.25" spans="1:2">
+    <row r="31" spans="1:4" ht="14.25">
       <c r="A31" s="27" t="s">
         <v>166</v>
       </c>
@@ -13759,8 +13157,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="21" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 20180521 Signed-off-by: MaHongTao <mht@shequchina.com>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_物件管理_駐車場.xlsx
+++ b/test_物件管理/test_物件管理_駐車場.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="850" firstSheet="7" activeTab="19"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="850" firstSheet="7" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="19" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="284">
   <si>
     <t>SQL</t>
   </si>
@@ -887,6 +887,9 @@
   </si>
   <si>
     <t>ホワイトボート</t>
+  </si>
+  <si>
+    <t>IN_DB_003</t>
   </si>
 </sst>
 </file>
@@ -905,8 +908,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1352,7 +1354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1387,7 +1389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -8257,6 +8259,9 @@
       <c r="B7" s="1" t="s">
         <v>254</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>255</v>
       </c>

</xml_diff>